<commit_message>
add solar simulation model, update simulation testbed
</commit_message>
<xml_diff>
--- a/PotatoPlanning/Cornell_Homer_electricity_sqm_consumption.xlsx
+++ b/PotatoPlanning/Cornell_Homer_electricity_sqm_consumption.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/yuancai_mit_edu/Documents/00Research/BaselinePrediction/Data/Cornell/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/yuancai_mit_edu/Documents/00Research/SimulationTestbed/PotatoPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EB942AD-958A-4DCB-B0A3-3677955FD1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{3EB942AD-958A-4DCB-B0A3-3677955FD1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4FA4C71-CA63-4232-B9D5-F7A9C82ED1E9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E6010009-1D8F-451C-915D-0EA3BBB5DBC6}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B2209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update model with control and temperature drift
</commit_message>
<xml_diff>
--- a/PotatoPlanning/Cornell_Homer_electricity_sqm_consumption.xlsx
+++ b/PotatoPlanning/Cornell_Homer_electricity_sqm_consumption.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/yuancai_mit_edu/Documents/00Research/SimulationTestbed/PotatoPlanning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{3EB942AD-958A-4DCB-B0A3-3677955FD1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4FA4C71-CA63-4232-B9D5-F7A9C82ED1E9}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{3EB942AD-958A-4DCB-B0A3-3677955FD1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34BFD606-FCAB-4A9B-B934-3BB30AC459A3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E6010009-1D8F-451C-915D-0EA3BBB5DBC6}"/>
+    <workbookView minimized="1" xWindow="5244" yWindow="3360" windowWidth="17280" windowHeight="8964" xr2:uid="{E6010009-1D8F-451C-915D-0EA3BBB5DBC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B2209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>